<commit_message>
new version of diploma
</commit_message>
<xml_diff>
--- a/СПЕКТРЫ/Обработка всех прошлых спектров/ОБРАБОТКА.xlsx
+++ b/СПЕКТРЫ/Обработка всех прошлых спектров/ОБРАБОТКА.xlsx
@@ -522,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -720,6 +720,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -753,11 +759,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1042,7 +1048,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E72" sqref="C67:E72"/>
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1089,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="73">
         <v>43851</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1104,7 +1110,7 @@
       <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1129,7 @@
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
@@ -1142,7 +1148,7 @@
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1167,7 @@
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
@@ -1180,7 +1186,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
@@ -1199,7 +1205,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1224,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1243,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1262,7 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
@@ -1275,7 +1281,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
@@ -1294,7 +1300,7 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
@@ -1313,7 +1319,7 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1338,7 @@
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="72"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +1357,7 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="72"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="15" t="s">
         <v>16</v>
       </c>
@@ -1370,7 +1376,7 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="72"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="15" t="s">
         <v>17</v>
       </c>
@@ -1389,7 +1395,7 @@
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="72"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="15" t="s">
         <v>18</v>
       </c>
@@ -1408,7 +1414,7 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="72"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="15" t="s">
         <v>19</v>
       </c>
@@ -1427,7 +1433,7 @@
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="72"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="15" t="s">
         <v>20</v>
       </c>
@@ -1446,7 +1452,7 @@
       <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="72"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="15" t="s">
         <v>21</v>
       </c>
@@ -1465,7 +1471,7 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="72"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="15" t="s">
         <v>22</v>
       </c>
@@ -1484,7 +1490,7 @@
       <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="72"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="15" t="s">
         <v>23</v>
       </c>
@@ -1503,7 +1509,7 @@
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="15" t="s">
         <v>24</v>
       </c>
@@ -1522,7 +1528,7 @@
       <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="15" t="s">
         <v>25</v>
       </c>
@@ -1541,7 +1547,7 @@
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="73"/>
+      <c r="A26" s="75"/>
       <c r="B26" s="16" t="s">
         <v>26</v>
       </c>
@@ -1560,7 +1566,7 @@
       <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="74">
+      <c r="A27" s="76">
         <v>44252</v>
       </c>
       <c r="B27" s="34" t="s">
@@ -1581,7 +1587,7 @@
       <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="75"/>
+      <c r="A28" s="77"/>
       <c r="B28" s="35" t="s">
         <v>3</v>
       </c>
@@ -1600,7 +1606,7 @@
       <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="75"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="35" t="s">
         <v>4</v>
       </c>
@@ -1619,7 +1625,7 @@
       <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="75"/>
+      <c r="A30" s="77"/>
       <c r="B30" s="35" t="s">
         <v>5</v>
       </c>
@@ -1638,7 +1644,7 @@
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="75"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="35" t="s">
         <v>6</v>
       </c>
@@ -1657,7 +1663,7 @@
       <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="75"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="35" t="s">
         <v>7</v>
       </c>
@@ -1676,7 +1682,7 @@
       <c r="G32" s="24"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="75"/>
+      <c r="A33" s="77"/>
       <c r="B33" s="35" t="s">
         <v>8</v>
       </c>
@@ -1695,7 +1701,7 @@
       <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="75"/>
+      <c r="A34" s="77"/>
       <c r="B34" s="35" t="s">
         <v>9</v>
       </c>
@@ -1712,15 +1718,15 @@
         <v>45</v>
       </c>
       <c r="G34" s="24"/>
-      <c r="I34" s="80" t="s">
+      <c r="I34" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="J34" s="80"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="80"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="75"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="35" t="s">
         <v>10</v>
       </c>
@@ -1751,7 +1757,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="75"/>
+      <c r="A36" s="77"/>
       <c r="B36" s="36" t="s">
         <v>11</v>
       </c>
@@ -1782,7 +1788,7 @@
       <c r="L36" s="68"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
+      <c r="A37" s="78"/>
       <c r="B37" s="30" t="s">
         <v>12</v>
       </c>
@@ -1813,7 +1819,7 @@
       <c r="L37" s="68"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
+      <c r="A38" s="78"/>
       <c r="B38" s="3" t="s">
         <v>13</v>
       </c>
@@ -1842,7 +1848,7 @@
       <c r="L38" s="68"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="76"/>
+      <c r="A39" s="78"/>
       <c r="B39" s="3" t="s">
         <v>14</v>
       </c>
@@ -1861,7 +1867,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
+      <c r="A40" s="78"/>
       <c r="B40" s="3" t="s">
         <v>15</v>
       </c>
@@ -1880,7 +1886,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="76"/>
+      <c r="A41" s="78"/>
       <c r="B41" s="3" t="s">
         <v>16</v>
       </c>
@@ -1899,7 +1905,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="76"/>
+      <c r="A42" s="78"/>
       <c r="B42" s="3" t="s">
         <v>17</v>
       </c>
@@ -1918,7 +1924,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="77"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="19" t="s">
         <v>18</v>
       </c>
@@ -1937,7 +1943,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="74">
+      <c r="A44" s="76">
         <v>44273</v>
       </c>
       <c r="B44" s="34" t="s">
@@ -1958,7 +1964,7 @@
       <c r="G44" s="29"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="78"/>
+      <c r="A45" s="80"/>
       <c r="B45" s="35" t="s">
         <v>3</v>
       </c>
@@ -1977,7 +1983,7 @@
       <c r="G45" s="24"/>
     </row>
     <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="78"/>
+      <c r="A46" s="80"/>
       <c r="B46" s="36" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2002,7 @@
       <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="72"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="30" t="s">
         <v>5</v>
       </c>
@@ -2015,7 +2021,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="72"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="3" t="s">
         <v>6</v>
       </c>
@@ -2034,7 +2040,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="72"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2053,7 +2059,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="72"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="3" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2078,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="72"/>
+      <c r="A51" s="74"/>
       <c r="B51" s="3" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2097,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="79"/>
+      <c r="A52" s="81"/>
       <c r="B52" s="38" t="s">
         <v>10</v>
       </c>
@@ -2110,7 +2116,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="74">
+      <c r="A53" s="76">
         <v>44280</v>
       </c>
       <c r="B53" s="47" t="s">
@@ -2129,7 +2135,7 @@
       <c r="G53" s="49"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="78"/>
+      <c r="A54" s="80"/>
       <c r="B54" s="45" t="s">
         <v>3</v>
       </c>
@@ -2146,7 +2152,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="78"/>
+      <c r="A55" s="80"/>
       <c r="B55" s="43" t="s">
         <v>4</v>
       </c>
@@ -2165,7 +2171,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="72"/>
+      <c r="A56" s="74"/>
       <c r="B56" s="46" t="s">
         <v>5</v>
       </c>
@@ -2182,7 +2188,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="78"/>
+      <c r="A57" s="80"/>
       <c r="B57" s="47" t="s">
         <v>6</v>
       </c>
@@ -2199,7 +2205,7 @@
       <c r="G57" s="49"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="72"/>
+      <c r="A58" s="74"/>
       <c r="B58" s="45" t="s">
         <v>7</v>
       </c>
@@ -2218,7 +2224,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="72"/>
+      <c r="A59" s="74"/>
       <c r="B59" s="43" t="s">
         <v>8</v>
       </c>
@@ -2235,7 +2241,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="72"/>
+      <c r="A60" s="74"/>
       <c r="B60" s="43" t="s">
         <v>9</v>
       </c>
@@ -2252,7 +2258,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="72"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="43" t="s">
         <v>10</v>
       </c>
@@ -2269,7 +2275,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="72"/>
+      <c r="A62" s="74"/>
       <c r="B62" s="43" t="s">
         <v>11</v>
       </c>
@@ -2288,7 +2294,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="72"/>
+      <c r="A63" s="74"/>
       <c r="B63" s="43" t="s">
         <v>12</v>
       </c>
@@ -2307,7 +2313,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="73"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="44" t="s">
         <v>13</v>
       </c>
@@ -2323,12 +2329,18 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C66" s="64"/>
       <c r="D66" s="64"/>
       <c r="E66" s="64"/>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="84">
+        <v>3300</v>
+      </c>
+      <c r="B67" s="84">
+        <v>50</v>
+      </c>
       <c r="C67" s="32">
         <v>656</v>
       </c>
@@ -2340,7 +2352,13 @@
       </c>
       <c r="F67" s="64"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="84">
+        <v>2600</v>
+      </c>
+      <c r="B68" s="84">
+        <v>250</v>
+      </c>
       <c r="C68" s="25">
         <v>890</v>
       </c>
@@ -2352,7 +2370,13 @@
       </c>
       <c r="F68" s="64"/>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="84">
+        <v>2600</v>
+      </c>
+      <c r="B69" s="84">
+        <v>450</v>
+      </c>
       <c r="C69" s="25">
         <v>654</v>
       </c>
@@ -2364,7 +2388,13 @@
       </c>
       <c r="F69" s="64"/>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="84">
+        <v>1600</v>
+      </c>
+      <c r="B70" s="84">
+        <v>650</v>
+      </c>
       <c r="C70" s="25">
         <v>658</v>
       </c>
@@ -2376,7 +2406,13 @@
       </c>
       <c r="F70" s="64"/>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="84">
+        <v>1200</v>
+      </c>
+      <c r="B71" s="84">
+        <v>850</v>
+      </c>
       <c r="C71" s="69">
         <v>1082</v>
       </c>
@@ -2388,7 +2424,13 @@
       </c>
       <c r="F71" s="64"/>
     </row>
-    <row r="72" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="84">
+        <v>800</v>
+      </c>
+      <c r="B72" s="84">
+        <v>1050</v>
+      </c>
       <c r="C72" s="11">
         <v>908</v>
       </c>
@@ -2400,69 +2442,129 @@
       </c>
       <c r="F72" s="64"/>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="82"/>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="84">
+        <v>400</v>
+      </c>
+      <c r="B73" s="84">
+        <v>1250</v>
+      </c>
+      <c r="C73" s="71"/>
       <c r="D73" s="9"/>
       <c r="E73" s="70">
         <v>165</v>
       </c>
     </row>
-    <row r="74" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="84">
+        <v>8.9540000000000006</v>
+      </c>
+      <c r="B74" s="84">
+        <v>2.3E-3</v>
+      </c>
       <c r="C74" s="62"/>
       <c r="D74" s="19"/>
       <c r="E74" s="63">
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C75" s="83"/>
+    <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="72"/>
       <c r="D75" s="48"/>
       <c r="E75" s="70">
         <v>176</v>
       </c>
     </row>
-    <row r="76" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="83"/>
+    <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="84">
+        <v>4000</v>
+      </c>
+      <c r="B76" s="84">
+        <v>50</v>
+      </c>
+      <c r="C76" s="72"/>
       <c r="D76" s="48"/>
       <c r="E76" s="70">
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="84">
+        <v>3600</v>
+      </c>
+      <c r="B77" s="84">
+        <v>650</v>
+      </c>
       <c r="C77" s="1"/>
       <c r="D77" s="69"/>
       <c r="E77" s="64"/>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="84">
+        <v>2300</v>
+      </c>
+      <c r="B78" s="84">
+        <v>1250</v>
+      </c>
       <c r="C78" s="1"/>
       <c r="D78" s="69"/>
       <c r="E78" s="64"/>
     </row>
-    <row r="79" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="84">
+        <v>1800</v>
+      </c>
+      <c r="B79" s="84">
+        <v>1850</v>
+      </c>
       <c r="C79" s="12"/>
       <c r="D79" s="11"/>
       <c r="E79" s="64"/>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="84">
+        <v>1400</v>
+      </c>
+      <c r="B80" s="84">
+        <v>2450</v>
+      </c>
       <c r="C80" s="63"/>
       <c r="D80" s="63"/>
       <c r="E80" s="64"/>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="84">
+        <v>1000</v>
+      </c>
+      <c r="B81" s="84">
+        <v>3050</v>
+      </c>
       <c r="C81" s="64"/>
       <c r="D81" s="64"/>
       <c r="E81" s="64"/>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="84">
+        <v>800</v>
+      </c>
+      <c r="B82" s="84">
+        <v>3650</v>
+      </c>
       <c r="E82" s="64"/>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="84">
+        <v>8.3170000000000002</v>
+      </c>
+      <c r="B83" s="85">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="E83" s="64"/>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E84" s="64"/>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E85" s="64"/>
     </row>
   </sheetData>
@@ -2498,12 +2600,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">

</xml_diff>